<commit_message>
Adding wiring tab to app
</commit_message>
<xml_diff>
--- a/Microclimate_data_supporting/MC_data_check_Elenter.xlsx
+++ b/Microclimate_data_supporting/MC_data_check_Elenter.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luky-my.sharepoint.com/personal/drva228_uky_edu/Documents/TMCF/Continuous_data/TMCF_Microclimate/Microclimate_data_supporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{3B37D695-BF22-4FAA-8AAF-9F7C225B7A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E58FF5A-E0C4-4D41-BEE3-65200FD7B3A8}"/>
+  <xr:revisionPtr revIDLastSave="671" documentId="8_{3B37D695-BF22-4FAA-8AAF-9F7C225B7A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2FA992E-32EE-4504-8701-7D0D3AE4ED0A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{91B74E48-8166-4C07-B8C8-350166F942B4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{91B74E48-8166-4C07-B8C8-350166F942B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Damon" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="119">
   <si>
     <t>Tree</t>
   </si>
@@ -69,13 +71,349 @@
   </si>
   <si>
     <t>Atmos_pressure</t>
+  </si>
+  <si>
+    <t>ET1</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>2022-10-31 09:15:00</t>
+  </si>
+  <si>
+    <t>2022-09-30 16:30:00 UTC</t>
+  </si>
+  <si>
+    <t>Espacio en blanco</t>
+  </si>
+  <si>
+    <t>2022-10-31 10:00:00</t>
+  </si>
+  <si>
+    <t>VPD</t>
+  </si>
+  <si>
+    <t>Wetness</t>
+  </si>
+  <si>
+    <t>2022-10-01 08:15:00</t>
+  </si>
+  <si>
+    <t>2022-10-31 22:15:00</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>2023-02-09 11:30:00</t>
+  </si>
+  <si>
+    <t>2023-03-08 13:30:00</t>
+  </si>
+  <si>
+    <t>Wind direction</t>
+  </si>
+  <si>
+    <t>2023-01-15 21:00:00</t>
+  </si>
+  <si>
+    <t>2023-01-16 13:30:00</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>2023-01-15 12:15:00</t>
+  </si>
+  <si>
+    <t>2023-01-16 11:00:00</t>
+  </si>
+  <si>
+    <t>Wind speed</t>
+  </si>
+  <si>
+    <t>2023-01-15 21:30:00</t>
+  </si>
+  <si>
+    <t>2023-01-16 13:15:00</t>
+  </si>
+  <si>
+    <t>Espacios separados</t>
+  </si>
+  <si>
+    <t>Gust speed</t>
+  </si>
+  <si>
+    <t>2022-09-30 15:15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-09-30 16:30:00 </t>
+  </si>
+  <si>
+    <t>ET1 Listo</t>
+  </si>
+  <si>
+    <t>FB2, 4,6, 8</t>
+  </si>
+  <si>
+    <t>TV4</t>
+  </si>
+  <si>
+    <t>Epifitas</t>
+  </si>
+  <si>
+    <t>ET8</t>
+  </si>
+  <si>
+    <t>Preguntar sobre wetness</t>
+  </si>
+  <si>
+    <t>solar, temp, RH, pressure, VPD, wetness, wind direction, wind speed, gust speed</t>
+  </si>
+  <si>
+    <t>ET2 Listo</t>
+  </si>
+  <si>
+    <t>ET3</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>2022-11-02 13:00:00</t>
+  </si>
+  <si>
+    <t>2022-11-23 10:15:00</t>
+  </si>
+  <si>
+    <t>2023-03-27 17:15:00</t>
+  </si>
+  <si>
+    <t>2023-04-12 12:30:00</t>
+  </si>
+  <si>
+    <t>2022-09-29 19:00:00</t>
+  </si>
+  <si>
+    <t>2022-11-23 09:15:00</t>
+  </si>
+  <si>
+    <t>2022-11-18 19:00:00</t>
+  </si>
+  <si>
+    <t>2022-11-23 10:45:00</t>
+  </si>
+  <si>
+    <t>2023-04-12 14:30:00</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>2023-01-28 08:00:00</t>
+  </si>
+  <si>
+    <t>2023-02-09 10:30:00</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>2022-11-18 17:30:00</t>
+  </si>
+  <si>
+    <t>2023-04-12 15:00:00</t>
+  </si>
+  <si>
+    <t>2023-02-09 10:45:00</t>
+  </si>
+  <si>
+    <t>2022-09-30 16:30:00</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>2022-09-30 16:15:00</t>
+  </si>
+  <si>
+    <t>2023-01-16 05:15:00</t>
+  </si>
+  <si>
+    <t>2022-10-31 11:15:00</t>
+  </si>
+  <si>
+    <t>2022-11-18 18:45:00</t>
+  </si>
+  <si>
+    <t>2022-11-23 10:30:00</t>
+  </si>
+  <si>
+    <t>2023-02-09 11:00:00</t>
+  </si>
+  <si>
+    <t>2023-03-27 16:00:00</t>
+  </si>
+  <si>
+    <t>2022-12-28 11:00:00</t>
+  </si>
+  <si>
+    <t>2023-01-01 20:45:00</t>
+  </si>
+  <si>
+    <t>2022-10-15 17:45:00</t>
+  </si>
+  <si>
+    <t>2022-11-23 14:45:00</t>
+  </si>
+  <si>
+    <t>2023-04-13 13:15:00</t>
+  </si>
+  <si>
+    <t>2022-09-06 12:30:00</t>
+  </si>
+  <si>
+    <t>2022-09-01</t>
+  </si>
+  <si>
+    <t>2023-04-12 16:00:00</t>
+  </si>
+  <si>
+    <t>2022-11-12 13:15:00</t>
+  </si>
+  <si>
+    <t>2022-11-23 12:45:00</t>
+  </si>
+  <si>
+    <t>2022-11-30 03:45:00</t>
+  </si>
+  <si>
+    <t>Datos extraños</t>
+  </si>
+  <si>
+    <t>2022-10-27 11:30:00</t>
+  </si>
+  <si>
+    <t>2022-10-27 18:00:00</t>
+  </si>
+  <si>
+    <t>Espacios separados y datos extraños</t>
+  </si>
+  <si>
+    <t>Espacios separados y datos extraños, el tubo largo estaba fallando</t>
+  </si>
+  <si>
+    <t>2022-12-21 18:30:00</t>
+  </si>
+  <si>
+    <t>2022-12-22 04:15:00</t>
+  </si>
+  <si>
+    <t>2023-01-11 12:30:00</t>
+  </si>
+  <si>
+    <t>2022-10-03 20:30:00</t>
+  </si>
+  <si>
+    <t>2022-10-10 09:15:00</t>
+  </si>
+  <si>
+    <t>2022-09-06 14:15:00</t>
+  </si>
+  <si>
+    <t>2023-04-12 16:45:00</t>
+  </si>
+  <si>
+    <t>2022-10-10 10:30:00</t>
+  </si>
+  <si>
+    <t>2022-09-06 13:15:00</t>
+  </si>
+  <si>
+    <t>solar, temp, RH, pressure, VPD, wetness, wind direction, wind speed,</t>
+  </si>
+  <si>
+    <t>Datalogger</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>MC1</t>
+  </si>
+  <si>
+    <t>Datalogger no funcionaba</t>
+  </si>
+  <si>
+    <t>Otra pagina</t>
+  </si>
+  <si>
+    <t>fila 9</t>
+  </si>
+  <si>
+    <t>filas en azul</t>
+  </si>
+  <si>
+    <t>MC2</t>
+  </si>
+  <si>
+    <t>filas en amarillo</t>
+  </si>
+  <si>
+    <t>fila 23</t>
+  </si>
+  <si>
+    <t>fila 21</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>filas en verde</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Espacios separados </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y datos raros</t>
+    </r>
+  </si>
+  <si>
+    <t>fila 42</t>
+  </si>
+  <si>
+    <t>fila 46</t>
+  </si>
+  <si>
+    <t>fila 47</t>
+  </si>
+  <si>
+    <t>fila 48</t>
+  </si>
+  <si>
+    <t>fila 49</t>
+  </si>
+  <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>filas en naranja</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,13 +421,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,9 +479,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -124,8 +509,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -441,19 +830,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94BC3E17-0F87-4847-8DFE-F4E0494DF5CB}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
     <col min="4" max="5" width="18" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -488,6 +877,1434 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24DD494-57E9-4B2C-AD03-DC71C7C4947F}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" customWidth="1"/>
+    <col min="6" max="7" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>